<commit_message>
2.4.5: Implement FUNCTION for DynamicClause.
</commit_message>
<xml_diff>
--- a/test/data/mysql/SampleMySQL004.xlsx
+++ b/test/data/mysql/SampleMySQL004.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/test/data/mysql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EA0ABB-4703-B443-A2F5-3883CEE2B4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB79CC9-6315-534C-B152-40A397E7A41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2520" windowWidth="33600" windowHeight="20540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4660" yWindow="2520" windowWidth="33600" windowHeight="20540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sql" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="190">
   <si>
     <t>パラメータ名</t>
     <rPh sb="5" eb="6">
@@ -1376,6 +1376,26 @@
   </si>
   <si>
     <t>funcLiteral</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FROM_UNIXTIME_DEFAULT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>OR test1.COL_DATE &lt; FROM_UNIXTIME( ?  )</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FUNC_LITERAL2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>funcLiteral2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   ${FUNC_LITERAL2}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2243,10 +2263,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M112"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2865,122 +2885,146 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="32"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="75"/>
+    <row r="35" spans="1:10" ht="30">
+      <c r="A35" s="32">
+        <f>A34+1</f>
+        <v>8</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>185</v>
+      </c>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
-      <c r="I35" s="69"/>
+      <c r="I35" s="69" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="32"/>
       <c r="B36" s="27"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
+      <c r="E36" s="75"/>
       <c r="F36" s="27"/>
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="I36" s="69"/>
     </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="17" t="s">
+    <row r="37" spans="1:10">
+      <c r="A37" s="32"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="69"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="35" t="s">
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="35" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="20" t="s">
+    <row r="40" spans="1:10" ht="45">
+      <c r="A40" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C40" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D40" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="E40" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F40" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="G40" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H39" s="21" t="s">
+      <c r="H40" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="I39" s="21" t="s">
+      <c r="I40" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="J39" s="70" t="s">
+      <c r="J40" s="70" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="30">
-      <c r="A40" s="76" t="s">
+    <row r="41" spans="1:10" ht="30">
+      <c r="A41" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B41" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="C40" s="78" t="s">
+      <c r="C41" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D41" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E41" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="F40" s="34" t="s">
+      <c r="F41" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="77"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="34"/>
-      <c r="J41" s="34"/>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="77"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
+      <c r="J41" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30">
+      <c r="A42" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C42" s="78" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>172</v>
+      </c>
       <c r="F42" s="34"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="J42" s="34" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="77"/>
@@ -2994,103 +3038,101 @@
       <c r="I43" s="34"/>
       <c r="J43" s="34"/>
     </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="17" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" s="77"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="64"/>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>0</v>
-      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
-      <c r="G46" s="35"/>
+      <c r="G46" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="H46" s="64"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="32"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="64"/>
+      <c r="A47" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="35"/>
       <c r="H47" s="64"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="28"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
       <c r="D48" s="30"/>
       <c r="E48" s="31"/>
       <c r="F48" s="65"/>
       <c r="G48" s="64"/>
       <c r="H48" s="64"/>
     </row>
-    <row r="50" spans="1:13">
-      <c r="A50" s="17" t="s">
+    <row r="49" spans="1:13">
+      <c r="A49" s="28"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="56"/>
-      <c r="J50" s="57"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="37" t="s">
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="57"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-      <c r="J51" s="59"/>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="60"/>
-      <c r="H52" s="60"/>
-      <c r="I52" s="60"/>
-      <c r="J52" s="61"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="58"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="59"/>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="42" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -3103,7 +3145,9 @@
       <c r="J53" s="61"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="42"/>
+      <c r="A54" s="42" t="s">
+        <v>124</v>
+      </c>
       <c r="B54" s="43"/>
       <c r="C54" s="43"/>
       <c r="D54" s="43"/>
@@ -3127,81 +3171,74 @@
       <c r="J55" s="61"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="47"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="63"/>
-    </row>
-    <row r="58" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A58" s="17" t="s">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="60"/>
+      <c r="J56" s="61"/>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="47"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="63"/>
+    </row>
+    <row r="59" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A59" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
-      <c r="I58" s="56"/>
-      <c r="J58" s="57"/>
-      <c r="K58" s="17" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L58" s="18"/>
-      <c r="M58" s="36"/>
-    </row>
-    <row r="59" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A59" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="74" t="s">
-        <v>117</v>
-      </c>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="59"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="40"/>
-      <c r="M59" s="41"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="36"/>
     </row>
     <row r="60" spans="1:13" ht="13.5" customHeight="1">
       <c r="A60" s="66" t="s">
-        <v>151</v>
-      </c>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="60"/>
-      <c r="I60" s="60"/>
-      <c r="J60" s="61"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="45"/>
-      <c r="M60" s="46"/>
+        <v>156</v>
+      </c>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="58"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="40"/>
+      <c r="M60" s="41"/>
     </row>
     <row r="61" spans="1:13" ht="13.5" customHeight="1">
       <c r="A61" s="66" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
-      <c r="D61" s="73" t="s">
-        <v>145</v>
-      </c>
+      <c r="D61" s="43"/>
       <c r="E61" s="43"/>
       <c r="F61" s="43"/>
       <c r="G61" s="60"/>
@@ -3214,15 +3251,15 @@
     </row>
     <row r="62" spans="1:13" ht="13.5" customHeight="1">
       <c r="A62" s="66" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="B62" s="43"/>
       <c r="C62" s="43"/>
       <c r="D62" s="73" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E62" s="43"/>
-      <c r="F62" s="73"/>
+      <c r="F62" s="43"/>
       <c r="G62" s="60"/>
       <c r="H62" s="60"/>
       <c r="I62" s="60"/>
@@ -3233,12 +3270,12 @@
     </row>
     <row r="63" spans="1:13" ht="13.5" customHeight="1">
       <c r="A63" s="66" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B63" s="43"/>
       <c r="C63" s="43"/>
       <c r="D63" s="73" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E63" s="43"/>
       <c r="F63" s="73"/>
@@ -3252,13 +3289,15 @@
     </row>
     <row r="64" spans="1:13" ht="13.5" customHeight="1">
       <c r="A64" s="66" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="B64" s="43"/>
       <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
+      <c r="D64" s="73" t="s">
+        <v>116</v>
+      </c>
       <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
+      <c r="F64" s="73"/>
       <c r="G64" s="60"/>
       <c r="H64" s="60"/>
       <c r="I64" s="60"/>
@@ -3269,7 +3308,7 @@
     </row>
     <row r="65" spans="1:13" ht="13.5" customHeight="1">
       <c r="A65" s="66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B65" s="43"/>
       <c r="C65" s="43"/>
@@ -3286,13 +3325,11 @@
     </row>
     <row r="66" spans="1:13" ht="13.5" customHeight="1">
       <c r="A66" s="66" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B66" s="43"/>
       <c r="C66" s="43"/>
-      <c r="D66" s="73" t="s">
-        <v>132</v>
-      </c>
+      <c r="D66" s="43"/>
       <c r="E66" s="43"/>
       <c r="F66" s="43"/>
       <c r="G66" s="60"/>
@@ -3305,12 +3342,12 @@
     </row>
     <row r="67" spans="1:13" ht="13.5" customHeight="1">
       <c r="A67" s="66" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="B67" s="43"/>
       <c r="C67" s="43"/>
       <c r="D67" s="73" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="E67" s="43"/>
       <c r="F67" s="43"/>
@@ -3324,7 +3361,7 @@
     </row>
     <row r="68" spans="1:13" ht="13.5" customHeight="1">
       <c r="A68" s="66" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="B68" s="43"/>
       <c r="C68" s="43"/>
@@ -3343,11 +3380,13 @@
     </row>
     <row r="69" spans="1:13" ht="13.5" customHeight="1">
       <c r="A69" s="66" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="B69" s="43"/>
       <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
+      <c r="D69" s="73" t="s">
+        <v>144</v>
+      </c>
       <c r="E69" s="43"/>
       <c r="F69" s="43"/>
       <c r="G69" s="60"/>
@@ -3359,10 +3398,14 @@
       <c r="M69" s="46"/>
     </row>
     <row r="70" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A70" s="66"/>
+      <c r="A70" s="66" t="s">
+        <v>189</v>
+      </c>
       <c r="B70" s="43"/>
       <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
+      <c r="D70" s="73" t="s">
+        <v>144</v>
+      </c>
       <c r="E70" s="43"/>
       <c r="F70" s="43"/>
       <c r="G70" s="60"/>
@@ -3374,7 +3417,9 @@
       <c r="M70" s="46"/>
     </row>
     <row r="71" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A71" s="66"/>
+      <c r="A71" s="66" t="s">
+        <v>141</v>
+      </c>
       <c r="B71" s="43"/>
       <c r="C71" s="43"/>
       <c r="D71" s="43"/>
@@ -3389,7 +3434,7 @@
       <c r="M71" s="46"/>
     </row>
     <row r="72" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A72" s="42"/>
+      <c r="A72" s="66"/>
       <c r="B72" s="43"/>
       <c r="C72" s="43"/>
       <c r="D72" s="43"/>
@@ -3404,7 +3449,7 @@
       <c r="M72" s="46"/>
     </row>
     <row r="73" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A73" s="42"/>
+      <c r="A73" s="66"/>
       <c r="B73" s="43"/>
       <c r="C73" s="43"/>
       <c r="D73" s="43"/>
@@ -3869,22 +3914,52 @@
       <c r="M103" s="46"/>
     </row>
     <row r="104" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A104" s="47"/>
-      <c r="B104" s="48"/>
-      <c r="C104" s="48"/>
-      <c r="D104" s="48"/>
-      <c r="E104" s="48"/>
-      <c r="F104" s="48"/>
-      <c r="G104" s="62"/>
-      <c r="H104" s="62"/>
-      <c r="I104" s="62"/>
-      <c r="J104" s="63"/>
-      <c r="K104" s="49"/>
-      <c r="L104" s="50"/>
-      <c r="M104" s="51"/>
-    </row>
-    <row r="111" spans="1:13" ht="13.5" customHeight="1"/>
-    <row r="112" spans="1:13" ht="13.5" customHeight="1"/>
+      <c r="A104" s="42"/>
+      <c r="B104" s="43"/>
+      <c r="C104" s="43"/>
+      <c r="D104" s="43"/>
+      <c r="E104" s="43"/>
+      <c r="F104" s="43"/>
+      <c r="G104" s="60"/>
+      <c r="H104" s="60"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="61"/>
+      <c r="K104" s="44"/>
+      <c r="L104" s="45"/>
+      <c r="M104" s="46"/>
+    </row>
+    <row r="105" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A105" s="42"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
+      <c r="E105" s="43"/>
+      <c r="F105" s="43"/>
+      <c r="G105" s="60"/>
+      <c r="H105" s="60"/>
+      <c r="I105" s="60"/>
+      <c r="J105" s="61"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="45"/>
+      <c r="M105" s="46"/>
+    </row>
+    <row r="106" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A106" s="47"/>
+      <c r="B106" s="48"/>
+      <c r="C106" s="48"/>
+      <c r="D106" s="48"/>
+      <c r="E106" s="48"/>
+      <c r="F106" s="48"/>
+      <c r="G106" s="62"/>
+      <c r="H106" s="62"/>
+      <c r="I106" s="62"/>
+      <c r="J106" s="63"/>
+      <c r="K106" s="49"/>
+      <c r="L106" s="50"/>
+      <c r="M106" s="51"/>
+    </row>
+    <row r="113" ht="13.5" customHeight="1"/>
+    <row r="114" ht="13.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <dataValidations count="11">
@@ -3894,7 +3969,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>SQLタイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C48 C18:C24 E40:I43" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C48:C49 C18:C24 E41:I44" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>パラメータタイプ</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
@@ -3909,16 +3984,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>入力パラメータBean</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D36" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28:D37" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>条件句タイプ</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F36" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28:F37" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>比較演算子</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28:G36" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28:G37" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>繰り返し時演算子</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J40:J43" xr:uid="{CEBFBCCE-1804-4841-A68F-7C7AC53D6F48}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J41:J44" xr:uid="{CEBFBCCE-1804-4841-A68F-7C7AC53D6F48}">
       <formula1>自動生成時チェック</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Just for recording: * add system properties.   -Dblanco.mysql.host : specify ip address of mysql server for generate sources.   -Dblanco.mysql.skip : specify false if you want to generate mysql test sources. * Remove duplicate argTimeout parameter from setInputStatement method. * Remove timestamp from resourcebundle.
</commit_message>
<xml_diff>
--- a/test/data/mysql/SampleMySQL004.xlsx
+++ b/test/data/mysql/SampleMySQL004.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbEE/test/data/mysql/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83320AA7-7234-3644-8FC3-1D54FE264C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F3FE9C-ED5E-8A49-B825-E50AD7850BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="2520" windowWidth="33600" windowHeight="20540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8020" yWindow="6460" windowWidth="33600" windowHeight="20540" tabRatio="457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sql" sheetId="38" r:id="rId1"/>
@@ -38,7 +38,6 @@
     <definedName name="論理演算子">config!$J$5:$J$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1763,7 +1762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1773,7 +1772,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1822,22 +1820,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1855,28 +1853,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1885,24 +1877,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1918,7 +1904,7 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1930,19 +1916,7 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1951,11 +1925,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1963,12 +1934,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2293,1715 +2258,1705 @@
   <dimension ref="A1:M115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="19.5" style="16" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" style="16" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="16"/>
+    <col min="1" max="1" width="5.1640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.5" style="15" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="J1" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="22"/>
+      <c r="E6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="27" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="27" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="27" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="27" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="27" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="27" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="36"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="52" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="36"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="53" t="s">
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="32">
+      <c r="A20" s="31">
         <f>A19+1</f>
         <v>2</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="53">
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="32">
         <v>12</v>
       </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="71"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="55"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="50"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="71"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="50"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="71"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="50"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="71"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="50"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="71"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="55"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="50"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="36"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="35"/>
     </row>
     <row r="28" spans="1:10" ht="28" customHeight="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="70" t="s">
+      <c r="G28" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J28" s="68"/>
+      <c r="J28" s="14"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27" t="s">
+      <c r="F29" s="26"/>
+      <c r="G29" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="69" t="s">
+      <c r="I29" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="J29" s="68"/>
+      <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="32">
+      <c r="A30" s="31">
         <f t="shared" ref="A30:A36" si="0">A29+1</f>
         <v>2</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27" t="s">
+      <c r="F30" s="26"/>
+      <c r="G30" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H30" s="27" t="s">
+      <c r="H30" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="69" t="s">
+      <c r="I30" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="J30" s="68"/>
+      <c r="J30" s="14"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="32">
+      <c r="A31" s="31">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="27" t="s">
+      <c r="G31" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H31" s="27" t="s">
+      <c r="H31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="69" t="s">
+      <c r="I31" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="J31" s="68" t="s">
+      <c r="J31" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="32">
+      <c r="A32" s="31">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="H32" s="27" t="s">
+      <c r="H32" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="69" t="s">
+      <c r="I32" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="J32" s="68"/>
+      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="32">
+      <c r="A33" s="31">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="69" t="s">
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="J33" s="68"/>
+      <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:10" ht="120">
-      <c r="A34" s="32">
+      <c r="A34" s="31">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="75" t="s">
+      <c r="E34" s="65" t="s">
         <v>159</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="68"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="14"/>
     </row>
     <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="32">
+      <c r="A35" s="31">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="D35" s="27" t="s">
+      <c r="D35" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="75" t="s">
+      <c r="E35" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="69" t="s">
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="60" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="32">
+      <c r="A36" s="31">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="26" t="s">
         <v>187</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="69" t="s">
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="60" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="32"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="69"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="60"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="32"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="69"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="60"/>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="35" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="34" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="F41" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="I41" s="21" t="s">
+      <c r="I41" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="J41" s="70" t="s">
+      <c r="J41" s="61" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30">
-      <c r="A42" s="76" t="s">
+      <c r="A42" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F42" s="34" t="s">
+      <c r="F42" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34" t="s">
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30">
-      <c r="A43" s="77" t="s">
+      <c r="A43" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="C43" s="78" t="s">
+      <c r="C43" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34" t="s">
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="77"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="33"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="77"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="35" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H47" s="64"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="64"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="34"/>
     </row>
     <row r="49" spans="1:13">
-      <c r="A49" s="32"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="50"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="28"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="50"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
-      <c r="J52" s="57"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="52"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="58"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="59"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="54"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="60"/>
-      <c r="H54" s="60"/>
-      <c r="I54" s="60"/>
-      <c r="J54" s="61"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="55"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="56"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="42" t="s">
+      <c r="A55" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="60"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="61"/>
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="56"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="42"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="60"/>
-      <c r="H56" s="60"/>
-      <c r="I56" s="60"/>
-      <c r="J56" s="61"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="55"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="55"/>
+      <c r="J56" s="56"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="42"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="43"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="60"/>
-      <c r="H57" s="60"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="61"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="56"/>
     </row>
     <row r="58" spans="1:13">
-      <c r="A58" s="47"/>
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="62"/>
-      <c r="H58" s="62"/>
-      <c r="I58" s="62"/>
-      <c r="J58" s="63"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="58"/>
     </row>
     <row r="60" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="17" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="52"/>
+      <c r="K60" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="L60" s="18"/>
-      <c r="M60" s="36"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="35"/>
     </row>
     <row r="61" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="B61" s="38"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="74" t="s">
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="59"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="40"/>
-      <c r="M61" s="41"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="38"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="40"/>
     </row>
     <row r="62" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="43"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="60"/>
-      <c r="J62" s="61"/>
-      <c r="K62" s="44"/>
-      <c r="L62" s="45"/>
-      <c r="M62" s="46"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="56"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="43"/>
     </row>
     <row r="63" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A63" s="66" t="s">
+      <c r="A63" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="B63" s="43"/>
-      <c r="C63" s="43"/>
-      <c r="D63" s="73" t="s">
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="60"/>
-      <c r="H63" s="60"/>
-      <c r="I63" s="60"/>
-      <c r="J63" s="61"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="45"/>
-      <c r="M63" s="46"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="55"/>
+      <c r="H63" s="55"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="56"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="43"/>
     </row>
     <row r="64" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A64" s="66" t="s">
+      <c r="A64" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="73" t="s">
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="E64" s="43"/>
-      <c r="F64" s="73"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
-      <c r="I64" s="60"/>
-      <c r="J64" s="61"/>
-      <c r="K64" s="44"/>
-      <c r="L64" s="45"/>
-      <c r="M64" s="46"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="55"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="43"/>
     </row>
     <row r="65" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A65" s="66" t="s">
+      <c r="A65" s="59" t="s">
         <v>152</v>
       </c>
-      <c r="B65" s="43"/>
-      <c r="C65" s="43"/>
-      <c r="D65" s="73" t="s">
+      <c r="B65" s="42"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="E65" s="43"/>
-      <c r="F65" s="73"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
-      <c r="J65" s="61"/>
-      <c r="K65" s="44"/>
-      <c r="L65" s="45"/>
-      <c r="M65" s="46"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="55"/>
+      <c r="I65" s="55"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="43"/>
     </row>
     <row r="66" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A66" s="66" t="s">
+      <c r="A66" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="61"/>
-      <c r="K66" s="44"/>
-      <c r="L66" s="45"/>
-      <c r="M66" s="46"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="55"/>
+      <c r="H66" s="55"/>
+      <c r="I66" s="55"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="43"/>
     </row>
     <row r="67" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B67" s="43"/>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="60"/>
-      <c r="H67" s="60"/>
-      <c r="I67" s="60"/>
-      <c r="J67" s="61"/>
-      <c r="K67" s="44"/>
-      <c r="L67" s="45"/>
-      <c r="M67" s="46"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="55"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="43"/>
     </row>
     <row r="68" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A68" s="66" t="s">
+      <c r="A68" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="43"/>
-      <c r="C68" s="43"/>
-      <c r="D68" s="73" t="s">
+      <c r="B68" s="42"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="E68" s="43"/>
-      <c r="F68" s="43"/>
-      <c r="G68" s="60"/>
-      <c r="H68" s="60"/>
-      <c r="I68" s="60"/>
-      <c r="J68" s="61"/>
-      <c r="K68" s="44"/>
-      <c r="L68" s="45"/>
-      <c r="M68" s="46"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="56"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="43"/>
     </row>
     <row r="69" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A69" s="66" t="s">
+      <c r="A69" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="43"/>
-      <c r="C69" s="43"/>
-      <c r="D69" s="73" t="s">
+      <c r="B69" s="42"/>
+      <c r="C69" s="42"/>
+      <c r="D69" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="60"/>
-      <c r="H69" s="60"/>
-      <c r="I69" s="60"/>
-      <c r="J69" s="61"/>
-      <c r="K69" s="44"/>
-      <c r="L69" s="45"/>
-      <c r="M69" s="46"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="55"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="43"/>
     </row>
     <row r="70" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A70" s="66" t="s">
+      <c r="A70" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="B70" s="43"/>
-      <c r="C70" s="43"/>
-      <c r="D70" s="73" t="s">
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="60"/>
-      <c r="H70" s="60"/>
-      <c r="I70" s="60"/>
-      <c r="J70" s="61"/>
-      <c r="K70" s="44"/>
-      <c r="L70" s="45"/>
-      <c r="M70" s="46"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="55"/>
+      <c r="H70" s="55"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="56"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="43"/>
     </row>
     <row r="71" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="59" t="s">
         <v>189</v>
       </c>
-      <c r="B71" s="43"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="73" t="s">
+      <c r="B71" s="42"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="60"/>
-      <c r="H71" s="60"/>
-      <c r="I71" s="60"/>
-      <c r="J71" s="61"/>
-      <c r="K71" s="44"/>
-      <c r="L71" s="45"/>
-      <c r="M71" s="46"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="55"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="56"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="43"/>
     </row>
     <row r="72" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A72" s="66" t="s">
+      <c r="A72" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="43"/>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="60"/>
-      <c r="H72" s="60"/>
-      <c r="I72" s="60"/>
-      <c r="J72" s="61"/>
-      <c r="K72" s="44"/>
-      <c r="L72" s="45"/>
-      <c r="M72" s="46"/>
+      <c r="B72" s="42"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="55"/>
+      <c r="I72" s="55"/>
+      <c r="J72" s="56"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="43"/>
     </row>
     <row r="73" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A73" s="66"/>
-      <c r="B73" s="43"/>
-      <c r="C73" s="43"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="60"/>
-      <c r="H73" s="60"/>
-      <c r="I73" s="60"/>
-      <c r="J73" s="61"/>
-      <c r="K73" s="44"/>
-      <c r="L73" s="45"/>
-      <c r="M73" s="46"/>
+      <c r="A73" s="59"/>
+      <c r="B73" s="42"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="55"/>
+      <c r="I73" s="55"/>
+      <c r="J73" s="56"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="43"/>
     </row>
     <row r="74" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A74" s="66"/>
-      <c r="B74" s="43"/>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
-      <c r="F74" s="43"/>
-      <c r="G74" s="60"/>
-      <c r="H74" s="60"/>
-      <c r="I74" s="60"/>
-      <c r="J74" s="61"/>
-      <c r="K74" s="44"/>
-      <c r="L74" s="45"/>
-      <c r="M74" s="46"/>
+      <c r="A74" s="59"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="55"/>
+      <c r="I74" s="55"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="43"/>
     </row>
     <row r="75" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A75" s="42"/>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="60"/>
-      <c r="H75" s="60"/>
-      <c r="I75" s="60"/>
-      <c r="J75" s="61"/>
-      <c r="K75" s="44"/>
-      <c r="L75" s="45"/>
-      <c r="M75" s="46"/>
+      <c r="A75" s="41"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
+      <c r="I75" s="55"/>
+      <c r="J75" s="56"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="43"/>
     </row>
     <row r="76" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A76" s="42"/>
-      <c r="B76" s="43"/>
-      <c r="C76" s="43"/>
-      <c r="D76" s="43"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="43"/>
-      <c r="G76" s="60"/>
-      <c r="H76" s="60"/>
-      <c r="I76" s="60"/>
-      <c r="J76" s="61"/>
-      <c r="K76" s="44"/>
-      <c r="L76" s="45"/>
-      <c r="M76" s="46"/>
+      <c r="A76" s="41"/>
+      <c r="B76" s="42"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="55"/>
+      <c r="I76" s="55"/>
+      <c r="J76" s="56"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="43"/>
     </row>
     <row r="77" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A77" s="42"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="43"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="60"/>
-      <c r="H77" s="60"/>
-      <c r="I77" s="60"/>
-      <c r="J77" s="61"/>
-      <c r="K77" s="44"/>
-      <c r="L77" s="45"/>
-      <c r="M77" s="46"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="55"/>
+      <c r="I77" s="55"/>
+      <c r="J77" s="56"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="43"/>
     </row>
     <row r="78" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A78" s="42"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="43"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="60"/>
-      <c r="H78" s="60"/>
-      <c r="I78" s="60"/>
-      <c r="J78" s="61"/>
-      <c r="K78" s="44"/>
-      <c r="L78" s="45"/>
-      <c r="M78" s="46"/>
+      <c r="A78" s="41"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="55"/>
+      <c r="I78" s="55"/>
+      <c r="J78" s="56"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="43"/>
     </row>
     <row r="79" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A79" s="42"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="43"/>
-      <c r="D79" s="43"/>
-      <c r="E79" s="43"/>
-      <c r="F79" s="43"/>
-      <c r="G79" s="60"/>
-      <c r="H79" s="60"/>
-      <c r="I79" s="60"/>
-      <c r="J79" s="61"/>
-      <c r="K79" s="44"/>
-      <c r="L79" s="45"/>
-      <c r="M79" s="46"/>
+      <c r="A79" s="41"/>
+      <c r="B79" s="42"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
+      <c r="G79" s="55"/>
+      <c r="H79" s="55"/>
+      <c r="I79" s="55"/>
+      <c r="J79" s="56"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="43"/>
     </row>
     <row r="80" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A80" s="42"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="60"/>
-      <c r="H80" s="60"/>
-      <c r="I80" s="60"/>
-      <c r="J80" s="61"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="45"/>
-      <c r="M80" s="46"/>
+      <c r="A80" s="41"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
+      <c r="F80" s="42"/>
+      <c r="G80" s="55"/>
+      <c r="H80" s="55"/>
+      <c r="I80" s="55"/>
+      <c r="J80" s="56"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="43"/>
     </row>
     <row r="81" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A81" s="42"/>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="43"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="60"/>
-      <c r="H81" s="60"/>
-      <c r="I81" s="60"/>
-      <c r="J81" s="61"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="45"/>
-      <c r="M81" s="46"/>
+      <c r="A81" s="41"/>
+      <c r="B81" s="42"/>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
+      <c r="F81" s="42"/>
+      <c r="G81" s="55"/>
+      <c r="H81" s="55"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="56"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="43"/>
     </row>
     <row r="82" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A82" s="42"/>
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="43"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="60"/>
-      <c r="H82" s="60"/>
-      <c r="I82" s="60"/>
-      <c r="J82" s="61"/>
-      <c r="K82" s="44"/>
-      <c r="L82" s="45"/>
-      <c r="M82" s="46"/>
+      <c r="A82" s="41"/>
+      <c r="B82" s="42"/>
+      <c r="C82" s="42"/>
+      <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
+      <c r="F82" s="42"/>
+      <c r="G82" s="55"/>
+      <c r="H82" s="55"/>
+      <c r="I82" s="55"/>
+      <c r="J82" s="56"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="43"/>
     </row>
     <row r="83" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A83" s="42"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
-      <c r="E83" s="43"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="60"/>
-      <c r="H83" s="60"/>
-      <c r="I83" s="60"/>
-      <c r="J83" s="61"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="45"/>
-      <c r="M83" s="46"/>
+      <c r="A83" s="41"/>
+      <c r="B83" s="42"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="55"/>
+      <c r="H83" s="55"/>
+      <c r="I83" s="55"/>
+      <c r="J83" s="56"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="43"/>
     </row>
     <row r="84" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A84" s="42"/>
-      <c r="B84" s="43"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="60"/>
-      <c r="I84" s="60"/>
-      <c r="J84" s="61"/>
-      <c r="K84" s="44"/>
-      <c r="L84" s="45"/>
-      <c r="M84" s="46"/>
+      <c r="A84" s="41"/>
+      <c r="B84" s="42"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
+      <c r="F84" s="42"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
+      <c r="I84" s="55"/>
+      <c r="J84" s="56"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="43"/>
     </row>
     <row r="85" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A85" s="42"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="43"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="60"/>
-      <c r="H85" s="60"/>
-      <c r="I85" s="60"/>
-      <c r="J85" s="61"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="45"/>
-      <c r="M85" s="46"/>
+      <c r="A85" s="41"/>
+      <c r="B85" s="42"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
+      <c r="F85" s="42"/>
+      <c r="G85" s="55"/>
+      <c r="H85" s="55"/>
+      <c r="I85" s="55"/>
+      <c r="J85" s="56"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="43"/>
     </row>
     <row r="86" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A86" s="42"/>
-      <c r="B86" s="43"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="60"/>
-      <c r="H86" s="60"/>
-      <c r="I86" s="60"/>
-      <c r="J86" s="61"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="45"/>
-      <c r="M86" s="46"/>
+      <c r="A86" s="41"/>
+      <c r="B86" s="42"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
+      <c r="F86" s="42"/>
+      <c r="G86" s="55"/>
+      <c r="H86" s="55"/>
+      <c r="I86" s="55"/>
+      <c r="J86" s="56"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="43"/>
     </row>
     <row r="87" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A87" s="42"/>
-      <c r="B87" s="43"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
-      <c r="G87" s="60"/>
-      <c r="H87" s="60"/>
-      <c r="I87" s="60"/>
-      <c r="J87" s="61"/>
-      <c r="K87" s="44"/>
-      <c r="L87" s="45"/>
-      <c r="M87" s="46"/>
+      <c r="A87" s="41"/>
+      <c r="B87" s="42"/>
+      <c r="C87" s="42"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
+      <c r="F87" s="42"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="55"/>
+      <c r="I87" s="55"/>
+      <c r="J87" s="56"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="43"/>
     </row>
     <row r="88" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A88" s="42"/>
-      <c r="B88" s="43"/>
-      <c r="C88" s="43"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="43"/>
-      <c r="F88" s="43"/>
-      <c r="G88" s="60"/>
-      <c r="H88" s="60"/>
-      <c r="I88" s="60"/>
-      <c r="J88" s="61"/>
-      <c r="K88" s="44"/>
-      <c r="L88" s="45"/>
-      <c r="M88" s="46"/>
+      <c r="A88" s="41"/>
+      <c r="B88" s="42"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
+      <c r="F88" s="42"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="55"/>
+      <c r="I88" s="55"/>
+      <c r="J88" s="56"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="43"/>
     </row>
     <row r="89" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A89" s="42"/>
-      <c r="B89" s="43"/>
-      <c r="C89" s="43"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43"/>
-      <c r="G89" s="60"/>
-      <c r="H89" s="60"/>
-      <c r="I89" s="60"/>
-      <c r="J89" s="61"/>
-      <c r="K89" s="44"/>
-      <c r="L89" s="45"/>
-      <c r="M89" s="46"/>
+      <c r="A89" s="41"/>
+      <c r="B89" s="42"/>
+      <c r="C89" s="42"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="55"/>
+      <c r="I89" s="55"/>
+      <c r="J89" s="56"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="43"/>
     </row>
     <row r="90" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A90" s="42"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="43"/>
-      <c r="E90" s="43"/>
-      <c r="F90" s="43"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="60"/>
-      <c r="I90" s="60"/>
-      <c r="J90" s="61"/>
-      <c r="K90" s="44"/>
-      <c r="L90" s="45"/>
-      <c r="M90" s="46"/>
+      <c r="A90" s="41"/>
+      <c r="B90" s="42"/>
+      <c r="C90" s="42"/>
+      <c r="D90" s="42"/>
+      <c r="E90" s="42"/>
+      <c r="F90" s="42"/>
+      <c r="G90" s="55"/>
+      <c r="H90" s="55"/>
+      <c r="I90" s="55"/>
+      <c r="J90" s="56"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="43"/>
     </row>
     <row r="91" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A91" s="42"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="43"/>
-      <c r="G91" s="60"/>
-      <c r="H91" s="60"/>
-      <c r="I91" s="60"/>
-      <c r="J91" s="61"/>
-      <c r="K91" s="44"/>
-      <c r="L91" s="45"/>
-      <c r="M91" s="46"/>
+      <c r="A91" s="41"/>
+      <c r="B91" s="42"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
+      <c r="F91" s="42"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="55"/>
+      <c r="I91" s="55"/>
+      <c r="J91" s="56"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="43"/>
     </row>
     <row r="92" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A92" s="42"/>
-      <c r="B92" s="43"/>
-      <c r="C92" s="43"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="60"/>
-      <c r="H92" s="60"/>
-      <c r="I92" s="60"/>
-      <c r="J92" s="61"/>
-      <c r="K92" s="44"/>
-      <c r="L92" s="45"/>
-      <c r="M92" s="46"/>
+      <c r="A92" s="41"/>
+      <c r="B92" s="42"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
+      <c r="F92" s="42"/>
+      <c r="G92" s="55"/>
+      <c r="H92" s="55"/>
+      <c r="I92" s="55"/>
+      <c r="J92" s="56"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="43"/>
     </row>
     <row r="93" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A93" s="42"/>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="60"/>
-      <c r="H93" s="60"/>
-      <c r="I93" s="60"/>
-      <c r="J93" s="61"/>
-      <c r="K93" s="44"/>
-      <c r="L93" s="45"/>
-      <c r="M93" s="46"/>
+      <c r="A93" s="41"/>
+      <c r="B93" s="42"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
+      <c r="F93" s="42"/>
+      <c r="G93" s="55"/>
+      <c r="H93" s="55"/>
+      <c r="I93" s="55"/>
+      <c r="J93" s="56"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="43"/>
     </row>
     <row r="94" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A94" s="42"/>
-      <c r="B94" s="43"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="43"/>
-      <c r="E94" s="43"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="60"/>
-      <c r="H94" s="60"/>
-      <c r="I94" s="60"/>
-      <c r="J94" s="61"/>
-      <c r="K94" s="44"/>
-      <c r="L94" s="45"/>
-      <c r="M94" s="46"/>
+      <c r="A94" s="41"/>
+      <c r="B94" s="42"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="55"/>
+      <c r="H94" s="55"/>
+      <c r="I94" s="55"/>
+      <c r="J94" s="56"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="43"/>
     </row>
     <row r="95" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A95" s="42"/>
-      <c r="B95" s="43"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="43"/>
-      <c r="E95" s="43"/>
-      <c r="F95" s="43"/>
-      <c r="G95" s="60"/>
-      <c r="H95" s="60"/>
-      <c r="I95" s="60"/>
-      <c r="J95" s="61"/>
-      <c r="K95" s="44"/>
-      <c r="L95" s="45"/>
-      <c r="M95" s="46"/>
+      <c r="A95" s="41"/>
+      <c r="B95" s="42"/>
+      <c r="C95" s="42"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="55"/>
+      <c r="H95" s="55"/>
+      <c r="I95" s="55"/>
+      <c r="J95" s="56"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="43"/>
     </row>
     <row r="96" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A96" s="42"/>
-      <c r="B96" s="43"/>
-      <c r="C96" s="43"/>
-      <c r="D96" s="43"/>
-      <c r="E96" s="43"/>
-      <c r="F96" s="43"/>
-      <c r="G96" s="60"/>
-      <c r="H96" s="60"/>
-      <c r="I96" s="60"/>
-      <c r="J96" s="61"/>
-      <c r="K96" s="44"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="46"/>
+      <c r="A96" s="41"/>
+      <c r="B96" s="42"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="55"/>
+      <c r="H96" s="55"/>
+      <c r="I96" s="55"/>
+      <c r="J96" s="56"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="43"/>
     </row>
     <row r="97" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A97" s="42"/>
-      <c r="B97" s="43"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="43"/>
-      <c r="E97" s="43"/>
-      <c r="F97" s="43"/>
-      <c r="G97" s="60"/>
-      <c r="H97" s="60"/>
-      <c r="I97" s="60"/>
-      <c r="J97" s="61"/>
-      <c r="K97" s="44"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="46"/>
+      <c r="A97" s="41"/>
+      <c r="B97" s="42"/>
+      <c r="C97" s="42"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
+      <c r="F97" s="42"/>
+      <c r="G97" s="55"/>
+      <c r="H97" s="55"/>
+      <c r="I97" s="55"/>
+      <c r="J97" s="56"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="43"/>
     </row>
     <row r="98" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A98" s="42"/>
-      <c r="B98" s="43"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="43"/>
-      <c r="E98" s="43"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="60"/>
-      <c r="H98" s="60"/>
-      <c r="I98" s="60"/>
-      <c r="J98" s="61"/>
-      <c r="K98" s="44"/>
-      <c r="L98" s="45"/>
-      <c r="M98" s="46"/>
+      <c r="A98" s="41"/>
+      <c r="B98" s="42"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
+      <c r="F98" s="42"/>
+      <c r="G98" s="55"/>
+      <c r="H98" s="55"/>
+      <c r="I98" s="55"/>
+      <c r="J98" s="56"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="43"/>
     </row>
     <row r="99" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A99" s="42"/>
-      <c r="B99" s="43"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="43"/>
-      <c r="E99" s="43"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="60"/>
-      <c r="H99" s="60"/>
-      <c r="I99" s="60"/>
-      <c r="J99" s="61"/>
-      <c r="K99" s="44"/>
-      <c r="L99" s="45"/>
-      <c r="M99" s="46"/>
+      <c r="A99" s="41"/>
+      <c r="B99" s="42"/>
+      <c r="C99" s="42"/>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
+      <c r="F99" s="42"/>
+      <c r="G99" s="55"/>
+      <c r="H99" s="55"/>
+      <c r="I99" s="55"/>
+      <c r="J99" s="56"/>
+      <c r="K99" s="18"/>
+      <c r="L99" s="14"/>
+      <c r="M99" s="43"/>
     </row>
     <row r="100" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A100" s="42"/>
-      <c r="B100" s="43"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-      <c r="E100" s="43"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="60"/>
-      <c r="H100" s="60"/>
-      <c r="I100" s="60"/>
-      <c r="J100" s="61"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="45"/>
-      <c r="M100" s="46"/>
+      <c r="A100" s="41"/>
+      <c r="B100" s="42"/>
+      <c r="C100" s="42"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
+      <c r="G100" s="55"/>
+      <c r="H100" s="55"/>
+      <c r="I100" s="55"/>
+      <c r="J100" s="56"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="43"/>
     </row>
     <row r="101" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A101" s="42"/>
-      <c r="B101" s="43"/>
-      <c r="C101" s="43"/>
-      <c r="D101" s="43"/>
-      <c r="E101" s="43"/>
-      <c r="F101" s="43"/>
-      <c r="G101" s="60"/>
-      <c r="H101" s="60"/>
-      <c r="I101" s="60"/>
-      <c r="J101" s="61"/>
-      <c r="K101" s="44"/>
-      <c r="L101" s="45"/>
-      <c r="M101" s="46"/>
+      <c r="A101" s="41"/>
+      <c r="B101" s="42"/>
+      <c r="C101" s="42"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
+      <c r="F101" s="42"/>
+      <c r="G101" s="55"/>
+      <c r="H101" s="55"/>
+      <c r="I101" s="55"/>
+      <c r="J101" s="56"/>
+      <c r="K101" s="18"/>
+      <c r="L101" s="14"/>
+      <c r="M101" s="43"/>
     </row>
     <row r="102" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A102" s="42"/>
-      <c r="B102" s="43"/>
-      <c r="C102" s="43"/>
-      <c r="D102" s="43"/>
-      <c r="E102" s="43"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="60"/>
-      <c r="H102" s="60"/>
-      <c r="I102" s="60"/>
-      <c r="J102" s="61"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="45"/>
-      <c r="M102" s="46"/>
+      <c r="A102" s="41"/>
+      <c r="B102" s="42"/>
+      <c r="C102" s="42"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
+      <c r="F102" s="42"/>
+      <c r="G102" s="55"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="55"/>
+      <c r="J102" s="56"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="14"/>
+      <c r="M102" s="43"/>
     </row>
     <row r="103" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A103" s="42"/>
-      <c r="B103" s="43"/>
-      <c r="C103" s="43"/>
-      <c r="D103" s="43"/>
-      <c r="E103" s="43"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="60"/>
-      <c r="H103" s="60"/>
-      <c r="I103" s="60"/>
-      <c r="J103" s="61"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="45"/>
-      <c r="M103" s="46"/>
+      <c r="A103" s="41"/>
+      <c r="B103" s="42"/>
+      <c r="C103" s="42"/>
+      <c r="D103" s="42"/>
+      <c r="E103" s="42"/>
+      <c r="F103" s="42"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="55"/>
+      <c r="J103" s="56"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="14"/>
+      <c r="M103" s="43"/>
     </row>
     <row r="104" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A104" s="42"/>
-      <c r="B104" s="43"/>
-      <c r="C104" s="43"/>
-      <c r="D104" s="43"/>
-      <c r="E104" s="43"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="60"/>
-      <c r="H104" s="60"/>
-      <c r="I104" s="60"/>
-      <c r="J104" s="61"/>
-      <c r="K104" s="44"/>
-      <c r="L104" s="45"/>
-      <c r="M104" s="46"/>
+      <c r="A104" s="41"/>
+      <c r="B104" s="42"/>
+      <c r="C104" s="42"/>
+      <c r="D104" s="42"/>
+      <c r="E104" s="42"/>
+      <c r="F104" s="42"/>
+      <c r="G104" s="55"/>
+      <c r="H104" s="55"/>
+      <c r="I104" s="55"/>
+      <c r="J104" s="56"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="14"/>
+      <c r="M104" s="43"/>
     </row>
     <row r="105" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A105" s="42"/>
-      <c r="B105" s="43"/>
-      <c r="C105" s="43"/>
-      <c r="D105" s="43"/>
-      <c r="E105" s="43"/>
-      <c r="F105" s="43"/>
-      <c r="G105" s="60"/>
-      <c r="H105" s="60"/>
-      <c r="I105" s="60"/>
-      <c r="J105" s="61"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="45"/>
-      <c r="M105" s="46"/>
+      <c r="A105" s="41"/>
+      <c r="B105" s="42"/>
+      <c r="C105" s="42"/>
+      <c r="D105" s="42"/>
+      <c r="E105" s="42"/>
+      <c r="F105" s="42"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="55"/>
+      <c r="J105" s="56"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="14"/>
+      <c r="M105" s="43"/>
     </row>
     <row r="106" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A106" s="42"/>
-      <c r="B106" s="43"/>
-      <c r="C106" s="43"/>
-      <c r="D106" s="43"/>
-      <c r="E106" s="43"/>
-      <c r="F106" s="43"/>
-      <c r="G106" s="60"/>
-      <c r="H106" s="60"/>
-      <c r="I106" s="60"/>
-      <c r="J106" s="61"/>
-      <c r="K106" s="44"/>
-      <c r="L106" s="45"/>
-      <c r="M106" s="46"/>
+      <c r="A106" s="41"/>
+      <c r="B106" s="42"/>
+      <c r="C106" s="42"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="55"/>
+      <c r="H106" s="55"/>
+      <c r="I106" s="55"/>
+      <c r="J106" s="56"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="14"/>
+      <c r="M106" s="43"/>
     </row>
     <row r="107" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A107" s="47"/>
-      <c r="B107" s="48"/>
-      <c r="C107" s="48"/>
-      <c r="D107" s="48"/>
-      <c r="E107" s="48"/>
-      <c r="F107" s="48"/>
-      <c r="G107" s="62"/>
-      <c r="H107" s="62"/>
-      <c r="I107" s="62"/>
-      <c r="J107" s="63"/>
-      <c r="K107" s="49"/>
-      <c r="L107" s="50"/>
-      <c r="M107" s="51"/>
+      <c r="A107" s="44"/>
+      <c r="B107" s="45"/>
+      <c r="C107" s="45"/>
+      <c r="D107" s="45"/>
+      <c r="E107" s="45"/>
+      <c r="F107" s="45"/>
+      <c r="G107" s="57"/>
+      <c r="H107" s="57"/>
+      <c r="I107" s="57"/>
+      <c r="J107" s="58"/>
+      <c r="K107" s="46"/>
+      <c r="L107" s="47"/>
+      <c r="M107" s="48"/>
     </row>
     <row r="114" ht="13.5" customHeight="1"/>
     <row r="115" ht="13.5" customHeight="1"/>
@@ -4078,7 +4033,7 @@
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4132,7 +4087,7 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -4158,210 +4113,186 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="8" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11" t="s">
+      <c r="C8" s="12"/>
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="72" t="s">
+      <c r="I9" s="62" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="5:5">
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="5:5">
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="5:5">
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="5:5">
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="5:5">
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="5:5">
-      <c r="E22" s="11"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="5:5">
-      <c r="E23" s="11"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="5:5">
-      <c r="E24" s="11"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="5:5">
-      <c r="E25" s="11"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="5:5">
-      <c r="E26" s="11"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="5:5">
-      <c r="E27" s="11"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="5:5">
-      <c r="E28" s="11"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="5:5">
-      <c r="E29" s="11"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="5:5">
-      <c r="E30" s="13"/>
+      <c r="E30" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>